<commit_message>
Adding a field to update input stock given in stockout task workflow
</commit_message>
<xml_diff>
--- a/forms/app/stockout.xlsx
+++ b/forms/app/stockout.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="141">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -418,7 +418,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-&lt;b&gt;ACT: ${requested_act} blisters&lt;/b&gt;</t>
+&lt;b&gt;Requested → ACT: ${requested_act} blisters&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -427,49 +427,210 @@
     <t xml:space="preserve">${act_was_selected} = ‘yes’</t>
   </si>
   <si>
+    <t xml:space="preserve">act_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT blisters given</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_zinc</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Zinc: ${requested_zinc} tablets&lt;/b&gt;</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Requested → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Zinc: ${requested_zinc} tablets&lt;/b&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${zinc_was_selected} = ‘yes’</t>
   </si>
   <si>
+    <t xml:space="preserve">zinc_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinc tablet given</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_amoxicillin</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Amoxicillin: ${requested_amoxicillin} tablets&lt;/b&gt;</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Requested → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Amoxicillin: ${requested_amoxicillin} tablets&lt;/b&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${amoxicillin_was_selected} = ‘yes’</t>
   </si>
   <si>
+    <t xml:space="preserve">amoxicillin_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amoxicillin tablets given</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_condoms</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Condoms: ${requested_condoms} pieces&lt;/b&gt;</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Requested → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Condoms: ${requested_condoms} pieces&lt;/b&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${condoms_was_selected} = ‘yes’</t>
   </si>
   <si>
+    <t xml:space="preserve">condoms_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condom pieces given</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_contraceptives</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Contraceptives: ${requested_contraceptives} tablets&lt;/b&gt;</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Requested → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Contraceptives: ${requested_contraceptives} tablets&lt;/b&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${contraceptives_was_selected} = ‘yes’</t>
   </si>
   <si>
+    <t xml:space="preserve">contraceptives_given </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contraceptives tablet given</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_sayana</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Sayana: ${requested_sayana} pieces &lt;/b&gt;</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Requested → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sayana: ${requested_sayana} pieces &lt;/b&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${sayana_was_selected} = ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sayana_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sayana Press pieces given</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -534,7 +695,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -589,6 +750,17 @@
       <name val="aakar"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFE36C09"/>
+      <name val="aakar"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="aakar"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -666,7 +838,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -727,15 +899,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,11 +1010,11 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2072,7 +2248,7 @@
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>96</v>
@@ -2083,8 +2259,8 @@
       <c r="D43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>98</v>
+      <c r="E43" s="14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,33 +2268,33 @@
         <v>89</v>
       </c>
       <c r="B44" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B45" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,64 +2302,157 @@
         <v>89</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E47" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-    </row>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+    </row>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2299,7 +2568,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
@@ -2308,83 +2577,83 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2409,34 +2678,34 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="17" t="n">
+        <v>139</v>
+      </c>
+      <c r="C2" s="18" t="n">
         <v>43880</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>